<commit_message>
August 2025 Readership Report
</commit_message>
<xml_diff>
--- a/Readership Reports/Places.xlsx
+++ b/Readership Reports/Places.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewmacpherson/development/GitHub/Readership-Word-Cloud/Readership Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE4896B-50CA-2545-846F-967BF61848D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60056108-2C93-0144-9CC6-CDEC3DE1DA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14260" windowHeight="15560" xr2:uid="{836667C0-DE47-B041-8E18-FB71019D3FBA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="340">
   <si>
     <t>Vancouver</t>
   </si>
@@ -1041,6 +1041,21 @@
   </si>
   <si>
     <t>Cangzhou, China</t>
+  </si>
+  <si>
+    <t>Joinville, Brazil</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>Santo Andre, Brazil</t>
+  </si>
+  <si>
+    <t>Sbcnet Ltda</t>
+  </si>
+  <si>
+    <t>Hangzhou, China</t>
   </si>
 </sst>
 </file>
@@ -1419,10 +1434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAC4019-EF2D-7E46-9CD0-5ADF4300B4E4}">
-  <dimension ref="A1:B318"/>
+  <dimension ref="A1:B322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A308" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B318" sqref="B318"/>
+    <sheetView tabSelected="1" topLeftCell="A306" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A324" sqref="A324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3074,6 +3089,29 @@
         <v>334</v>
       </c>
     </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A319" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A320" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B321" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>